<commit_message>
New page and new Features
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\ben\Documents\EcoFly-Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEA99D0-5E27-42EB-8737-40BCB2ECD769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9191A20-AC40-49BF-9F34-6939DD430F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{394786C6-30BE-4EE2-82C5-08B82B755672}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{394786C6-30BE-4EE2-82C5-08B82B755672}"/>
   </bookViews>
   <sheets>
     <sheet name="Short_Haul" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="95">
   <si>
     <t>Destination</t>
   </si>
@@ -322,7 +322,10 @@
     <t>Cargo (t)</t>
   </si>
   <si>
-    <t>Fuel/y (t)</t>
+    <t>Fuel  (t)</t>
+  </si>
+  <si>
+    <t>Fuel/y</t>
   </si>
 </sst>
 </file>
@@ -332,7 +335,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -474,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -972,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04E9B01-3FF7-45BE-B1FF-B37D4E1C4953}">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,17 +991,18 @@
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>87</v>
       </c>
@@ -1021,38 +1025,41 @@
       <c r="H1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>13</v>
       </c>
@@ -1078,46 +1085,50 @@
       <c r="H2" s="3">
         <v>2174</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
+        <f>G2*H2</f>
+        <v>3174040</v>
+      </c>
+      <c r="J2" s="4">
         <f>'[1]CO2 calculations'!K3</f>
         <v>8348.16</v>
       </c>
-      <c r="J2" s="4">
-        <f t="shared" ref="J2:J15" si="1">I2*G2</f>
+      <c r="K2" s="4">
+        <f t="shared" ref="K2:K15" si="1">J2*G2</f>
         <v>12188313.6</v>
       </c>
-      <c r="K2" s="4">
-        <f t="shared" ref="K2:K15" si="2">J2*(3.16/3.84)</f>
+      <c r="L2" s="4">
+        <f t="shared" ref="L2:L15" si="2">K2*(3.16/3.84)</f>
         <v>10029966.4</v>
       </c>
-      <c r="L2" s="4">
-        <f t="shared" ref="L2:L15" si="3">J2-K2</f>
+      <c r="M2" s="4">
+        <f t="shared" ref="M2:M15" si="3">K2-L2</f>
         <v>2158347.1999999993</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>150</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C3</f>
         <v>55560.000000000007</v>
       </c>
-      <c r="O2" s="5">
-        <f>N2*G2</f>
+      <c r="P2" s="5">
+        <f t="shared" ref="P2:P15" si="4">O2*G2</f>
         <v>81117600.000000015</v>
       </c>
-      <c r="P2" s="6">
-        <f>N2*0.8</f>
+      <c r="Q2" s="6">
+        <f>O2*0.8</f>
         <v>44448.000000000007</v>
       </c>
-      <c r="Q2" s="5">
-        <f>O2*0.8</f>
+      <c r="R2" s="5">
+        <f>P2*0.8</f>
         <v>64894080.000000015</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
@@ -1143,46 +1154,50 @@
       <c r="H3" s="9">
         <v>2873.2</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I15" si="5">G3*H3</f>
+        <v>2097436</v>
+      </c>
+      <c r="J3" s="10">
         <f>'[1]CO2 calculations'!K4</f>
         <v>11033.088</v>
       </c>
-      <c r="J3" s="10">
+      <c r="K3" s="10">
         <f t="shared" si="1"/>
         <v>8054154.2400000002</v>
       </c>
-      <c r="K3" s="11">
+      <c r="L3" s="11">
         <f t="shared" si="2"/>
         <v>6627897.7600000007</v>
       </c>
-      <c r="L3" s="11">
+      <c r="M3" s="11">
         <f t="shared" si="3"/>
         <v>1426256.4799999995</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>150</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C4</f>
         <v>73061.400000000009</v>
       </c>
-      <c r="O3" s="12">
-        <f>N3*G3</f>
+      <c r="P3" s="12">
+        <f t="shared" si="4"/>
         <v>53334822.000000007</v>
       </c>
-      <c r="P3" s="14">
-        <f>N3*0.8</f>
+      <c r="Q3" s="14">
+        <f>O3*0.8</f>
         <v>58449.12000000001</v>
       </c>
-      <c r="Q3" s="12">
-        <f t="shared" ref="Q3:Q15" si="4">O3*0.8</f>
+      <c r="R3" s="12">
+        <f t="shared" ref="R3:R15" si="6">P3*0.8</f>
         <v>42667857.600000009</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>13</v>
       </c>
@@ -1208,46 +1223,50 @@
       <c r="H4" s="3">
         <v>4620.3</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
+        <f t="shared" si="5"/>
+        <v>1441533.6</v>
+      </c>
+      <c r="J4" s="4">
         <f>'[1]CO2 calculations'!K5</f>
         <v>17741.952000000001</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <f t="shared" si="1"/>
         <v>5535489.0240000002</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <f t="shared" si="2"/>
         <v>4555246.1760000009</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <f t="shared" si="3"/>
         <v>980242.8479999993</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>150</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C5</f>
         <v>172791.6</v>
       </c>
-      <c r="O4" s="5">
-        <f>N4*G4</f>
+      <c r="P4" s="5">
+        <f t="shared" si="4"/>
         <v>53910979.200000003</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" ref="P4:P15" si="5">N4*0.8</f>
+      <c r="Q4" s="6">
+        <f t="shared" ref="Q4:Q15" si="7">O4*0.8</f>
         <v>138233.28</v>
       </c>
-      <c r="Q4" s="5">
-        <f t="shared" si="4"/>
+      <c r="R4" s="5">
+        <f t="shared" si="6"/>
         <v>43128783.360000007</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>20000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
@@ -1273,46 +1292,50 @@
       <c r="H5" s="9">
         <v>2982.2249999999999</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="3">
+        <f t="shared" si="5"/>
+        <v>930454.2</v>
+      </c>
+      <c r="J5" s="10">
         <f>'[1]CO2 calculations'!K6</f>
         <v>11451.743999999999</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="10">
         <f t="shared" si="1"/>
         <v>3572944.1279999996</v>
       </c>
-      <c r="K5" s="11">
+      <c r="L5" s="11">
         <f t="shared" si="2"/>
         <v>2940235.2719999999</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="11">
         <f t="shared" si="3"/>
         <v>632708.85599999968</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>150</v>
       </c>
-      <c r="N5" s="12">
+      <c r="O5" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C6</f>
         <v>95007.6</v>
       </c>
-      <c r="O5" s="12">
-        <f>N5*G5</f>
+      <c r="P5" s="12">
+        <f t="shared" si="4"/>
         <v>29642371.200000003</v>
       </c>
-      <c r="P5" s="14">
-        <f t="shared" si="5"/>
+      <c r="Q5" s="14">
+        <f t="shared" si="7"/>
         <v>76006.080000000002</v>
       </c>
-      <c r="Q5" s="12">
-        <f t="shared" si="4"/>
+      <c r="R5" s="12">
+        <f t="shared" si="6"/>
         <v>23713896.960000005</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>20000</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>13</v>
       </c>
@@ -1338,46 +1361,50 @@
       <c r="H6" s="3">
         <v>2802.7249999999999</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
+        <f t="shared" si="5"/>
+        <v>2045989.25</v>
+      </c>
+      <c r="J6" s="4">
         <f>'[1]CO2 calculations'!K7</f>
         <v>10762.464</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <f t="shared" si="1"/>
         <v>7856598.7199999997</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <f t="shared" si="2"/>
         <v>6465326.0300000003</v>
       </c>
-      <c r="L6" s="4">
+      <c r="M6" s="4">
         <f t="shared" si="3"/>
         <v>1391272.6899999995</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>150</v>
       </c>
-      <c r="N6" s="5">
+      <c r="O6" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C7</f>
         <v>88896</v>
       </c>
-      <c r="O6" s="5">
-        <f>N6*G6</f>
+      <c r="P6" s="5">
+        <f t="shared" si="4"/>
         <v>64894080</v>
       </c>
-      <c r="P6" s="6">
-        <f t="shared" si="5"/>
+      <c r="Q6" s="6">
+        <f t="shared" si="7"/>
         <v>71116.800000000003</v>
       </c>
-      <c r="Q6" s="5">
-        <f t="shared" si="4"/>
+      <c r="R6" s="5">
+        <f t="shared" si="6"/>
         <v>51915264</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>13</v>
       </c>
@@ -1403,46 +1430,50 @@
       <c r="H7" s="9">
         <v>2126.2249999999999</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="3">
+        <f t="shared" si="5"/>
+        <v>663382.19999999995</v>
+      </c>
+      <c r="J7" s="10">
         <f>'[1]CO2 calculations'!K8</f>
         <v>8164.7039999999997</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="10">
         <f t="shared" si="1"/>
         <v>2547387.648</v>
       </c>
-      <c r="K7" s="11">
+      <c r="L7" s="11">
         <f t="shared" si="2"/>
         <v>2096287.7520000003</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M7" s="11">
         <f t="shared" si="3"/>
         <v>451099.89599999972</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>150</v>
       </c>
-      <c r="N7" s="12">
+      <c r="O7" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C8</f>
         <v>56949.000000000007</v>
       </c>
-      <c r="O7" s="12">
-        <f>N7*G7</f>
+      <c r="P7" s="12">
+        <f t="shared" si="4"/>
         <v>17768088.000000004</v>
       </c>
-      <c r="P7" s="14">
-        <f t="shared" si="5"/>
+      <c r="Q7" s="14">
+        <f t="shared" si="7"/>
         <v>45559.200000000012</v>
       </c>
-      <c r="Q7" s="12">
-        <f t="shared" si="4"/>
+      <c r="R7" s="12">
+        <f t="shared" si="6"/>
         <v>14214470.400000004</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>20000</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
@@ -1468,46 +1499,50 @@
       <c r="H8" s="3">
         <v>1486.35</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
+        <f t="shared" si="5"/>
+        <v>463741.19999999995</v>
+      </c>
+      <c r="J8" s="4">
         <f>'[1]CO2 calculations'!K9</f>
         <v>5707.5839999999998</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <f t="shared" si="1"/>
         <v>1780766.2079999999</v>
       </c>
-      <c r="K8" s="4">
+      <c r="L8" s="4">
         <f t="shared" si="2"/>
         <v>1465422.192</v>
       </c>
-      <c r="L8" s="4">
+      <c r="M8" s="4">
         <f t="shared" si="3"/>
         <v>315344.01599999983</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>150</v>
       </c>
-      <c r="N8" s="5">
+      <c r="O8" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C9</f>
         <v>34447.200000000004</v>
       </c>
-      <c r="O8" s="5">
-        <f>N8*G8</f>
+      <c r="P8" s="5">
+        <f t="shared" si="4"/>
         <v>10747526.400000002</v>
       </c>
-      <c r="P8" s="6">
-        <f t="shared" si="5"/>
+      <c r="Q8" s="6">
+        <f t="shared" si="7"/>
         <v>27557.760000000006</v>
       </c>
-      <c r="Q8" s="5">
-        <f t="shared" si="4"/>
+      <c r="R8" s="5">
+        <f t="shared" si="6"/>
         <v>8598021.1200000029</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>13</v>
       </c>
@@ -1533,46 +1568,50 @@
       <c r="H9" s="9">
         <v>3010.7750000000001</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="3">
+        <f t="shared" si="5"/>
+        <v>2197865.75</v>
+      </c>
+      <c r="J9" s="10">
         <f>'[1]CO2 calculations'!K10</f>
         <v>11561.376</v>
       </c>
-      <c r="J9" s="10">
+      <c r="K9" s="10">
         <f t="shared" si="1"/>
         <v>8439804.4800000004</v>
       </c>
-      <c r="K9" s="11">
+      <c r="L9" s="11">
         <f t="shared" si="2"/>
         <v>6945255.7700000014</v>
       </c>
-      <c r="L9" s="11">
+      <c r="M9" s="11">
         <f t="shared" si="3"/>
         <v>1494548.709999999</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>150</v>
       </c>
-      <c r="N9" s="12">
+      <c r="O9" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C10</f>
         <v>99730.200000000012</v>
       </c>
-      <c r="O9" s="12">
-        <f>N9*G9</f>
+      <c r="P9" s="12">
+        <f t="shared" si="4"/>
         <v>72803046.000000015</v>
       </c>
-      <c r="P9" s="14">
-        <f t="shared" si="5"/>
+      <c r="Q9" s="14">
+        <f t="shared" si="7"/>
         <v>79784.160000000018</v>
       </c>
-      <c r="Q9" s="12">
-        <f t="shared" si="4"/>
+      <c r="R9" s="12">
+        <f t="shared" si="6"/>
         <v>58242436.800000012</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>20000</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
@@ -1598,46 +1637,50 @@
       <c r="H10" s="3">
         <v>2274.7249999999999</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
+        <f t="shared" si="5"/>
+        <v>3321098.5</v>
+      </c>
+      <c r="J10" s="4">
         <f>'[1]CO2 calculations'!K11</f>
         <v>8734.9439999999995</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <f t="shared" si="1"/>
         <v>12753018.239999998</v>
       </c>
-      <c r="K10" s="4">
+      <c r="L10" s="4">
         <f t="shared" si="2"/>
         <v>10494671.26</v>
       </c>
-      <c r="L10" s="4">
+      <c r="M10" s="4">
         <f t="shared" si="3"/>
         <v>2258346.9799999986</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>150</v>
       </c>
-      <c r="N10" s="5">
+      <c r="O10" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C11</f>
         <v>59727</v>
       </c>
-      <c r="O10" s="5">
-        <f>N10*G10</f>
+      <c r="P10" s="5">
+        <f t="shared" si="4"/>
         <v>87201420</v>
       </c>
-      <c r="P10" s="6">
-        <f t="shared" si="5"/>
+      <c r="Q10" s="6">
+        <f t="shared" si="7"/>
         <v>47781.600000000006</v>
       </c>
-      <c r="Q10" s="5">
-        <f t="shared" si="4"/>
+      <c r="R10" s="5">
+        <f t="shared" si="6"/>
         <v>69761136</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>20000</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>13</v>
       </c>
@@ -1663,46 +1706,50 @@
       <c r="H11" s="9">
         <v>4227.6750000000002</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="3">
+        <f t="shared" si="5"/>
+        <v>1319034.6000000001</v>
+      </c>
+      <c r="J11" s="10">
         <f>'[1]CO2 calculations'!K12</f>
         <v>16234.272000000001</v>
       </c>
-      <c r="J11" s="10">
+      <c r="K11" s="10">
         <f t="shared" si="1"/>
         <v>5065092.8640000001</v>
       </c>
-      <c r="K11" s="11">
+      <c r="L11" s="11">
         <f t="shared" si="2"/>
         <v>4168149.3360000006</v>
       </c>
-      <c r="L11" s="11">
+      <c r="M11" s="11">
         <f t="shared" si="3"/>
         <v>896943.52799999947</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>150</v>
       </c>
-      <c r="N11" s="12">
+      <c r="O11" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C12</f>
         <v>148067.40000000002</v>
       </c>
-      <c r="O11" s="12">
-        <f>N11*G11</f>
+      <c r="P11" s="12">
+        <f t="shared" si="4"/>
         <v>46197028.800000004</v>
       </c>
-      <c r="P11" s="14">
-        <f t="shared" si="5"/>
+      <c r="Q11" s="14">
+        <f t="shared" si="7"/>
         <v>118453.92000000003</v>
       </c>
-      <c r="Q11" s="12">
-        <f t="shared" si="4"/>
+      <c r="R11" s="12">
+        <f t="shared" si="6"/>
         <v>36957623.040000007</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>20000</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1728,46 +1775,50 @@
       <c r="H12" s="3">
         <v>3588.125</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
+        <f t="shared" si="5"/>
+        <v>1119495</v>
+      </c>
+      <c r="J12" s="4">
         <f>'[1]CO2 calculations'!K13</f>
         <v>13778.4</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <f t="shared" si="1"/>
         <v>4298860.8</v>
       </c>
-      <c r="K12" s="4">
+      <c r="L12" s="4">
         <f t="shared" si="2"/>
         <v>3537604.2</v>
       </c>
-      <c r="L12" s="4">
+      <c r="M12" s="4">
         <f t="shared" si="3"/>
         <v>761256.59999999963</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>150</v>
       </c>
-      <c r="N12" s="5">
+      <c r="O12" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C13</f>
         <v>119454</v>
       </c>
-      <c r="O12" s="5">
-        <f>N12*G12</f>
+      <c r="P12" s="5">
+        <f t="shared" si="4"/>
         <v>37269648</v>
       </c>
-      <c r="P12" s="6">
-        <f t="shared" si="5"/>
+      <c r="Q12" s="6">
+        <f t="shared" si="7"/>
         <v>95563.200000000012</v>
       </c>
-      <c r="Q12" s="5">
-        <f t="shared" si="4"/>
+      <c r="R12" s="5">
+        <f t="shared" si="6"/>
         <v>29815718.400000002</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>20000</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>13</v>
       </c>
@@ -1793,46 +1844,50 @@
       <c r="H13" s="9">
         <v>5185.3999999999996</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="3">
+        <f t="shared" si="5"/>
+        <v>3785341.9999999995</v>
+      </c>
+      <c r="J13" s="10">
         <f>'[1]CO2 calculations'!K14</f>
         <v>19911.935999999998</v>
       </c>
-      <c r="J13" s="10">
+      <c r="K13" s="10">
         <f t="shared" si="1"/>
         <v>14535713.279999999</v>
       </c>
-      <c r="K13" s="11">
+      <c r="L13" s="11">
         <f t="shared" si="2"/>
         <v>11961680.720000001</v>
       </c>
-      <c r="L13" s="11">
+      <c r="M13" s="11">
         <f t="shared" si="3"/>
         <v>2574032.5599999987</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>150</v>
       </c>
-      <c r="N13" s="12">
+      <c r="O13" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C14</f>
         <v>194460</v>
       </c>
-      <c r="O13" s="12">
-        <f>N13*G13</f>
+      <c r="P13" s="12">
+        <f t="shared" si="4"/>
         <v>141955800</v>
       </c>
-      <c r="P13" s="14">
-        <f t="shared" si="5"/>
+      <c r="Q13" s="14">
+        <f t="shared" si="7"/>
         <v>155568</v>
       </c>
-      <c r="Q13" s="12">
-        <f t="shared" si="4"/>
+      <c r="R13" s="12">
+        <f t="shared" si="6"/>
         <v>113564640</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>20000</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>13</v>
       </c>
@@ -1858,46 +1913,50 @@
       <c r="H14" s="3">
         <v>6247.125</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
+        <f t="shared" si="5"/>
+        <v>4560401.25</v>
+      </c>
+      <c r="J14" s="4">
         <f>'[1]CO2 calculations'!K15</f>
         <v>23988.959999999999</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <f t="shared" si="1"/>
         <v>17511940.800000001</v>
       </c>
-      <c r="K14" s="4">
+      <c r="L14" s="4">
         <f t="shared" si="2"/>
         <v>14410867.950000001</v>
       </c>
-      <c r="L14" s="4">
+      <c r="M14" s="4">
         <f t="shared" si="3"/>
         <v>3101072.8499999996</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>150</v>
       </c>
-      <c r="N14" s="5">
+      <c r="O14" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C15</f>
         <v>219184.2</v>
       </c>
-      <c r="O14" s="5">
-        <f>N14*G14</f>
+      <c r="P14" s="5">
+        <f t="shared" si="4"/>
         <v>160004466</v>
       </c>
-      <c r="P14" s="6">
-        <f t="shared" si="5"/>
+      <c r="Q14" s="6">
+        <f t="shared" si="7"/>
         <v>175347.36000000002</v>
       </c>
-      <c r="Q14" s="5">
-        <f t="shared" si="4"/>
+      <c r="R14" s="5">
+        <f t="shared" si="6"/>
         <v>128003572.80000001</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>20000</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>13</v>
       </c>
@@ -1923,42 +1982,46 @@
       <c r="H15" s="9">
         <v>5268.8</v>
       </c>
-      <c r="I15" s="10">
+      <c r="I15" s="3">
+        <f t="shared" si="5"/>
+        <v>3846224</v>
+      </c>
+      <c r="J15" s="10">
         <f>'[1]CO2 calculations'!K16</f>
         <v>20232.191999999999</v>
       </c>
-      <c r="J15" s="10">
+      <c r="K15" s="10">
         <f t="shared" si="1"/>
         <v>14769500.16</v>
       </c>
-      <c r="K15" s="11">
+      <c r="L15" s="11">
         <f t="shared" si="2"/>
         <v>12154067.840000002</v>
       </c>
-      <c r="L15" s="11">
+      <c r="M15" s="11">
         <f t="shared" si="3"/>
         <v>2615432.3199999984</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>150</v>
       </c>
-      <c r="N15" s="12">
+      <c r="O15" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C16</f>
         <v>186126.00000000003</v>
       </c>
-      <c r="O15" s="12">
-        <f>N15*G15</f>
+      <c r="P15" s="12">
+        <f t="shared" si="4"/>
         <v>135871980.00000003</v>
       </c>
-      <c r="P15" s="14">
-        <f t="shared" si="5"/>
+      <c r="Q15" s="14">
+        <f t="shared" si="7"/>
         <v>148900.80000000002</v>
       </c>
-      <c r="Q15" s="12">
-        <f t="shared" si="4"/>
+      <c r="R15" s="12">
+        <f t="shared" si="6"/>
         <v>108697584.00000003</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>20000</v>
       </c>
     </row>
@@ -1969,10 +2032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F7E59F-12D8-455D-83B7-BC2E9A7794EF}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1984,17 +2047,18 @@
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>87</v>
       </c>
@@ -2017,38 +2081,41 @@
       <c r="H1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>60</v>
       </c>
@@ -2074,38 +2141,42 @@
       <c r="H2" s="3">
         <v>103992.37</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
+        <f>G2*H2</f>
+        <v>32445619.439999998</v>
+      </c>
+      <c r="J2" s="4">
         <v>399330.70079999999</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <v>124591178.6496</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>102528157.43040001</v>
       </c>
-      <c r="L2" s="4">
+      <c r="M2" s="4">
         <v>22063021.219199985</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>301</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <v>1719304.2</v>
       </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <v>536422910.39999998</v>
       </c>
-      <c r="P2" s="6">
+      <c r="Q2" s="6">
         <v>1375443</v>
       </c>
-      <c r="Q2" s="5">
+      <c r="R2" s="5">
         <v>429138328</v>
       </c>
-      <c r="R2" s="5">
+      <c r="S2" s="5">
         <v>50000</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>60</v>
       </c>
@@ -2131,38 +2202,42 @@
       <c r="H3" s="9">
         <v>83634.09</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I7" si="1">G3*H3</f>
+        <v>26093836.079999998</v>
+      </c>
+      <c r="J3" s="10">
         <v>321154.9056</v>
       </c>
-      <c r="J3" s="10">
+      <c r="K3" s="10">
         <v>100200330.54719999</v>
       </c>
-      <c r="K3" s="11">
+      <c r="L3" s="11">
         <v>82456522.012800008</v>
       </c>
-      <c r="L3" s="11">
+      <c r="M3" s="11">
         <v>17743808.534399986</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>301</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>1326217.2</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>413779766.39999998</v>
       </c>
-      <c r="P3" s="13">
+      <c r="Q3" s="13">
         <v>1060973</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>331023813</v>
       </c>
-      <c r="R3" s="5">
+      <c r="S3" s="5">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>60</v>
       </c>
@@ -2188,38 +2263,42 @@
       <c r="H4" s="3">
         <v>108618.22</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>11296294.880000001</v>
+      </c>
+      <c r="J4" s="4">
         <v>417093.96480000002</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <v>43377772.339200005</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <v>35696291.820800006</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>7681480.5183999985</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>301</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>1748751</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>181870104</v>
       </c>
-      <c r="P4" s="6">
+      <c r="Q4" s="6">
         <v>1399000</v>
       </c>
-      <c r="Q4" s="5">
+      <c r="R4" s="5">
         <v>145496083</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <v>50000</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>60</v>
       </c>
@@ -2245,38 +2324,42 @@
       <c r="H5" s="9">
         <v>95974.47</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>29944034.640000001</v>
+      </c>
+      <c r="J5" s="10">
         <v>368541.96480000002</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="10">
         <v>114985093.0176</v>
       </c>
-      <c r="K5" s="11">
+      <c r="L5" s="11">
         <v>94623149.462400004</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="11">
         <v>20361943.555199996</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>301</v>
       </c>
-      <c r="N5" s="12">
+      <c r="O5" s="12">
         <v>1703191.8</v>
       </c>
-      <c r="O5" s="12">
+      <c r="P5" s="12">
         <v>531395841.60000002</v>
       </c>
-      <c r="P5" s="13">
+      <c r="Q5" s="13">
         <v>1362553</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="R5" s="12">
         <v>425116673</v>
       </c>
-      <c r="R5" s="5">
+      <c r="S5" s="5">
         <v>50000</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>60</v>
       </c>
@@ -2302,38 +2385,42 @@
       <c r="H6" s="3">
         <v>74692.789999999994</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>23304150.479999997</v>
+      </c>
+      <c r="J6" s="4">
         <v>286820.31359999994</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>89487937.843199983</v>
       </c>
-      <c r="K6" s="4">
+      <c r="L6" s="4">
         <v>73641115.516799986</v>
       </c>
-      <c r="L6" s="4">
+      <c r="M6" s="4">
         <v>15846822.326399997</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>301</v>
       </c>
-      <c r="N6" s="5">
+      <c r="O6" s="5">
         <v>1382055</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <v>431201160</v>
       </c>
-      <c r="P6" s="6">
+      <c r="Q6" s="6">
         <v>1105644</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="R6" s="5">
         <v>344960928</v>
       </c>
-      <c r="R6" s="5">
+      <c r="S6" s="5">
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>60</v>
       </c>
@@ -2359,36 +2446,64 @@
       <c r="H7" s="9">
         <v>75655.91</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>7868214.6400000006</v>
+      </c>
+      <c r="J7" s="10">
         <v>290518.69439999998</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="10">
         <v>30213944.217599999</v>
       </c>
-      <c r="K7" s="11">
+      <c r="L7" s="11">
         <v>24863558.262400001</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M7" s="11">
         <v>5350385.9551999979</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>301</v>
       </c>
-      <c r="N7" s="12">
+      <c r="O7" s="12">
         <v>1185094.8</v>
       </c>
-      <c r="O7" s="12">
+      <c r="P7" s="12">
         <v>123249859.2</v>
       </c>
-      <c r="P7" s="13">
+      <c r="Q7" s="13">
         <v>948075</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="R7" s="12">
         <v>98599887</v>
       </c>
-      <c r="R7" s="5">
+      <c r="S7" s="5">
         <v>50000</v>
       </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2399,11 +2514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFD40EF-32B6-43D3-9528-BB87908E07F7}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2445,8 +2563,8 @@
         <v>9172</v>
       </c>
       <c r="D2" s="20">
-        <f>48867.6/1000</f>
-        <v>48.867599999999996</v>
+        <f>SUM(Short_Haul!I:I)/1000</f>
+        <v>30966.037550000001</v>
       </c>
       <c r="E2">
         <v>97.85</v>
@@ -2458,11 +2576,11 @@
         <v>118.91</v>
       </c>
       <c r="H2">
-        <f>SUM(Short_Haul!M2:M15)*2</f>
+        <f>SUM(Short_Haul!N2:N15)*2</f>
         <v>4200</v>
       </c>
       <c r="I2">
-        <f>SUM(Short_Haul!R2:R15)/1000</f>
+        <f>SUM(Short_Haul!S2:S15)/1000</f>
         <v>280</v>
       </c>
     </row>
@@ -2477,8 +2595,8 @@
         <v>1456</v>
       </c>
       <c r="D3" s="20">
-        <f>542567.9/1000</f>
-        <v>542.56790000000001</v>
+        <f>SUM(Long_Haul!I:I)/1000</f>
+        <v>130952.15015999998</v>
       </c>
       <c r="E3">
         <v>413.81</v>
@@ -2490,11 +2608,11 @@
         <v>502.86</v>
       </c>
       <c r="H3">
-        <f>SUM(Long_Haul!M2:M7)*2</f>
+        <f>SUM(Long_Haul!N2:N7)*2</f>
         <v>3612</v>
       </c>
       <c r="I3">
-        <f>SUM(Long_Haul!R2:R7)/1000</f>
+        <f>SUM(Long_Haul!S2:S7)/1000</f>
         <v>300</v>
       </c>
     </row>
@@ -2510,7 +2628,7 @@
       </c>
       <c r="D4" s="20">
         <f>SUM(D2:D3)</f>
-        <v>591.43550000000005</v>
+        <v>161918.18770999997</v>
       </c>
       <c r="E4">
         <v>511.66</v>

</xml_diff>

<commit_message>
First 4am commit ever
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\ben\Documents\EcoFly-Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D6C5D5-B4AE-44DD-AC46-7DA9566A438C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FE6DF4-6100-4163-BC51-04DF8CF04192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{394786C6-30BE-4EE2-82C5-08B82B755672}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{394786C6-30BE-4EE2-82C5-08B82B755672}"/>
   </bookViews>
   <sheets>
     <sheet name="Short_Haul" sheetId="1" r:id="rId1"/>
     <sheet name="Long_Haul" sheetId="2" r:id="rId2"/>
     <sheet name="Dash" sheetId="3" r:id="rId3"/>
     <sheet name="PLUS MINUS" sheetId="4" r:id="rId4"/>
+    <sheet name="KPI" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="122">
   <si>
     <t>Destination</t>
   </si>
@@ -366,16 +367,60 @@
   </si>
   <si>
     <t>SAF Feasibility</t>
+  </si>
+  <si>
+    <t>Baseline 2025</t>
+  </si>
+  <si>
+    <t>Total Fuel</t>
+  </si>
+  <si>
+    <t>Total Emissions in kton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Available Seats </t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Technical feasibility</t>
+  </si>
+  <si>
+    <t>Legislation</t>
+  </si>
+  <si>
+    <t>Safety</t>
+  </si>
+  <si>
+    <t>Profit Margin</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Fleet Renewal 2050</t>
+  </si>
+  <si>
+    <t>SAF Utilization 2050</t>
+  </si>
+  <si>
+    <t>Revenue per Year</t>
+  </si>
+  <si>
+    <t>Lithium 2050</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -453,12 +498,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -532,11 +579,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2712,7 +2767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38507096-A2D6-4CA6-BE66-A9E3858283FE}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2841,4 +2896,210 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4771372-8E57-4810-B6F7-53ADB8BB6C1D}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="27">
+        <v>161918</v>
+      </c>
+      <c r="C2" s="27">
+        <f>B2*0.8</f>
+        <v>129534.40000000001</v>
+      </c>
+      <c r="D2" s="27">
+        <f>B2</f>
+        <v>161918</v>
+      </c>
+      <c r="E2" s="27">
+        <f>B2</f>
+        <v>161918</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>675.83</v>
+      </c>
+      <c r="C3">
+        <v>337.91</v>
+      </c>
+      <c r="D3">
+        <v>337.91</v>
+      </c>
+      <c r="E3">
+        <v>337.91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4">
+        <v>1814056</v>
+      </c>
+      <c r="C4">
+        <v>2109600</v>
+      </c>
+      <c r="D4">
+        <v>1814056</v>
+      </c>
+      <c r="E4">
+        <v>1814056</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="29">
+        <f>299887.98*10268</f>
+        <v>3079249778.6399999</v>
+      </c>
+      <c r="C8" s="29">
+        <f>4080000000+B8</f>
+        <v>7159249778.6399994</v>
+      </c>
+      <c r="D8" s="30">
+        <f>536143503.15+B8</f>
+        <v>3615393281.79</v>
+      </c>
+      <c r="E8" s="31">
+        <f>2117627480.85+B8</f>
+        <v>5196877259.4899998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="31">
+        <f>343760*10268</f>
+        <v>3529727680</v>
+      </c>
+      <c r="C9" s="31">
+        <f t="shared" ref="C9:E9" si="0">343760*10268</f>
+        <v>3529727680</v>
+      </c>
+      <c r="D9" s="31">
+        <f t="shared" si="0"/>
+        <v>3529727680</v>
+      </c>
+      <c r="E9" s="31">
+        <f t="shared" si="0"/>
+        <v>3529727680</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="32">
+        <f>(B9-B8)/B9</f>
+        <v>0.12762398184780083</v>
+      </c>
+      <c r="C10" s="32">
+        <f>(C9-C8)/C9</f>
+        <v>-1.0282725546238172</v>
+      </c>
+      <c r="D10" s="32">
+        <f t="shared" ref="D10:E10" si="1">(D9-D8)/D9</f>
+        <v>-2.426974813819064E-2</v>
+      </c>
+      <c r="E10" s="32">
+        <f t="shared" si="1"/>
+        <v>-0.47231677076289347</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create new branch and Dashboard
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\ben\Documents\EcoFly-Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F8BFD0-9CBA-478B-A10D-5612A63322FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E4B1E5-48BB-4106-984F-9C259542BDE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{394786C6-30BE-4EE2-82C5-08B82B755672}"/>
   </bookViews>
@@ -312,9 +312,6 @@
     <t>Seats</t>
   </si>
   <si>
-    <t>Cargo</t>
-  </si>
-  <si>
     <t>Seats/y</t>
   </si>
   <si>
@@ -418,18 +415,22 @@
   </si>
   <si>
     <t>Total CO2e</t>
+  </si>
+  <si>
+    <t>Cargo/y (kg)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_ [$€-2]\ * #,##0.00_ ;_ [$€-2]\ * \-#,##0.00_ ;_ [$€-2]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -514,7 +515,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -591,6 +592,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1093,7 +1097,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I2" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,16 +1109,16 @@
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -1137,41 +1141,41 @@
       <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1197,50 +1201,52 @@
         <f t="shared" ref="G2:G15" si="0">IF(F2="day",(E2*365*2),(E2*52*2))</f>
         <v>1460</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2">
+        <f t="shared" ref="H2:H15" si="1">150*G2</f>
+        <v>219000</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I15" si="2">20000*G2</f>
+        <v>29200000</v>
+      </c>
+      <c r="J2" s="3">
         <v>2174</v>
       </c>
-      <c r="I2" s="3">
-        <f>G2*H2</f>
+      <c r="K2" s="3">
+        <f>G2*J2</f>
         <v>3174040</v>
       </c>
-      <c r="J2" s="4">
+      <c r="L2" s="4">
         <f>'[1]CO2 calculations'!K3</f>
         <v>8348.16</v>
       </c>
-      <c r="K2" s="4">
-        <f t="shared" ref="K2:K15" si="1">J2*G2</f>
+      <c r="M2" s="4">
+        <f t="shared" ref="M2:M15" si="3">L2*G2</f>
         <v>12188313.6</v>
       </c>
-      <c r="L2" s="4">
-        <f t="shared" ref="L2:L15" si="2">K2*(3.16/3.84)</f>
+      <c r="N2" s="4">
+        <f t="shared" ref="N2:N15" si="4">M2*(3.16/3.84)</f>
         <v>10029966.4</v>
       </c>
-      <c r="M2" s="4">
-        <f t="shared" ref="M2:M15" si="3">K2-L2</f>
+      <c r="O2" s="4">
+        <f t="shared" ref="O2:O15" si="5">M2-N2</f>
         <v>2158347.1999999993</v>
       </c>
-      <c r="N2">
-        <v>150</v>
-      </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C3</f>
         <v>55560.000000000007</v>
       </c>
-      <c r="P2" s="5">
-        <f t="shared" ref="P2:P15" si="4">O2*G2</f>
+      <c r="Q2" s="5">
+        <f t="shared" ref="Q2:Q15" si="6">P2*G2</f>
         <v>81117600.000000015</v>
       </c>
-      <c r="Q2" s="6">
-        <f>O2*0.8</f>
+      <c r="R2" s="6">
+        <f>P2*0.8</f>
         <v>44448.000000000007</v>
       </c>
-      <c r="R2" s="5">
-        <f>P2*0.8</f>
+      <c r="S2" s="5">
+        <f>Q2*0.8</f>
         <v>64894080.000000015</v>
-      </c>
-      <c r="S2">
-        <v>20000</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -1266,50 +1272,52 @@
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3">
+        <f t="shared" si="1"/>
+        <v>109500</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="2"/>
+        <v>14600000</v>
+      </c>
+      <c r="J3" s="9">
         <v>2873.2</v>
       </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I15" si="5">G3*H3</f>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K15" si="7">G3*J3</f>
         <v>2097436</v>
       </c>
-      <c r="J3" s="10">
+      <c r="L3" s="10">
         <f>'[1]CO2 calculations'!K4</f>
         <v>11033.088</v>
       </c>
-      <c r="K3" s="10">
-        <f t="shared" si="1"/>
+      <c r="M3" s="10">
+        <f t="shared" si="3"/>
         <v>8054154.2400000002</v>
       </c>
-      <c r="L3" s="11">
-        <f t="shared" si="2"/>
+      <c r="N3" s="11">
+        <f t="shared" si="4"/>
         <v>6627897.7600000007</v>
       </c>
-      <c r="M3" s="11">
-        <f t="shared" si="3"/>
+      <c r="O3" s="11">
+        <f t="shared" si="5"/>
         <v>1426256.4799999995</v>
       </c>
-      <c r="N3">
-        <v>150</v>
-      </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C4</f>
         <v>73061.400000000009</v>
       </c>
-      <c r="P3" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q3" s="12">
+        <f t="shared" si="6"/>
         <v>53334822.000000007</v>
       </c>
-      <c r="Q3" s="14">
-        <f>O3*0.8</f>
+      <c r="R3" s="14">
+        <f>P3*0.8</f>
         <v>58449.12000000001</v>
       </c>
-      <c r="R3" s="12">
-        <f t="shared" ref="R3:R15" si="6">P3*0.8</f>
+      <c r="S3" s="12">
+        <f t="shared" ref="S3:S15" si="8">Q3*0.8</f>
         <v>42667857.600000009</v>
-      </c>
-      <c r="S3">
-        <v>20000</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -1335,50 +1343,52 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>46800</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="2"/>
+        <v>6240000</v>
+      </c>
+      <c r="J4" s="3">
         <v>4620.3</v>
       </c>
-      <c r="I4" s="3">
-        <f t="shared" si="5"/>
+      <c r="K4" s="3">
+        <f t="shared" si="7"/>
         <v>1441533.6</v>
       </c>
-      <c r="J4" s="4">
+      <c r="L4" s="4">
         <f>'[1]CO2 calculations'!K5</f>
         <v>17741.952000000001</v>
       </c>
-      <c r="K4" s="4">
-        <f t="shared" si="1"/>
-        <v>5535489.0240000002</v>
-      </c>
-      <c r="L4" s="4">
-        <f t="shared" si="2"/>
-        <v>4555246.1760000009</v>
-      </c>
       <c r="M4" s="4">
         <f t="shared" si="3"/>
+        <v>5535489.0240000002</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="4"/>
+        <v>4555246.1760000009</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="5"/>
         <v>980242.8479999993</v>
       </c>
-      <c r="N4">
-        <v>150</v>
-      </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C5</f>
         <v>172791.6</v>
       </c>
-      <c r="P4" s="5">
-        <f t="shared" si="4"/>
+      <c r="Q4" s="5">
+        <f t="shared" si="6"/>
         <v>53910979.200000003</v>
       </c>
-      <c r="Q4" s="6">
-        <f t="shared" ref="Q4:Q15" si="7">O4*0.8</f>
+      <c r="R4" s="6">
+        <f t="shared" ref="R4:R15" si="9">P4*0.8</f>
         <v>138233.28</v>
       </c>
-      <c r="R4" s="5">
-        <f t="shared" si="6"/>
+      <c r="S4" s="5">
+        <f t="shared" si="8"/>
         <v>43128783.360000007</v>
-      </c>
-      <c r="S4">
-        <v>20000</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1404,50 +1414,52 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>46800</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>6240000</v>
+      </c>
+      <c r="J5" s="9">
         <v>2982.2249999999999</v>
       </c>
-      <c r="I5" s="3">
-        <f t="shared" si="5"/>
+      <c r="K5" s="3">
+        <f t="shared" si="7"/>
         <v>930454.2</v>
       </c>
-      <c r="J5" s="10">
+      <c r="L5" s="10">
         <f>'[1]CO2 calculations'!K6</f>
         <v>11451.743999999999</v>
       </c>
-      <c r="K5" s="10">
-        <f t="shared" si="1"/>
+      <c r="M5" s="10">
+        <f t="shared" si="3"/>
         <v>3572944.1279999996</v>
       </c>
-      <c r="L5" s="11">
-        <f t="shared" si="2"/>
+      <c r="N5" s="11">
+        <f t="shared" si="4"/>
         <v>2940235.2719999999</v>
       </c>
-      <c r="M5" s="11">
-        <f t="shared" si="3"/>
+      <c r="O5" s="11">
+        <f t="shared" si="5"/>
         <v>632708.85599999968</v>
       </c>
-      <c r="N5">
-        <v>150</v>
-      </c>
-      <c r="O5" s="12">
+      <c r="P5" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C6</f>
         <v>95007.6</v>
       </c>
-      <c r="P5" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q5" s="12">
+        <f t="shared" si="6"/>
         <v>29642371.200000003</v>
       </c>
-      <c r="Q5" s="14">
-        <f t="shared" si="7"/>
+      <c r="R5" s="14">
+        <f t="shared" si="9"/>
         <v>76006.080000000002</v>
       </c>
-      <c r="R5" s="12">
-        <f t="shared" si="6"/>
+      <c r="S5" s="12">
+        <f t="shared" si="8"/>
         <v>23713896.960000005</v>
-      </c>
-      <c r="S5">
-        <v>20000</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -1473,50 +1485,52 @@
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>109500</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>14600000</v>
+      </c>
+      <c r="J6" s="3">
         <v>2802.7249999999999</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" si="5"/>
+      <c r="K6" s="3">
+        <f t="shared" si="7"/>
         <v>2045989.25</v>
       </c>
-      <c r="J6" s="4">
+      <c r="L6" s="4">
         <f>'[1]CO2 calculations'!K7</f>
         <v>10762.464</v>
       </c>
-      <c r="K6" s="4">
-        <f t="shared" si="1"/>
-        <v>7856598.7199999997</v>
-      </c>
-      <c r="L6" s="4">
-        <f t="shared" si="2"/>
-        <v>6465326.0300000003</v>
-      </c>
       <c r="M6" s="4">
         <f t="shared" si="3"/>
+        <v>7856598.7199999997</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="4"/>
+        <v>6465326.0300000003</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="5"/>
         <v>1391272.6899999995</v>
       </c>
-      <c r="N6">
-        <v>150</v>
-      </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C7</f>
         <v>88896</v>
       </c>
-      <c r="P6" s="5">
-        <f t="shared" si="4"/>
+      <c r="Q6" s="5">
+        <f t="shared" si="6"/>
         <v>64894080</v>
       </c>
-      <c r="Q6" s="6">
-        <f t="shared" si="7"/>
+      <c r="R6" s="6">
+        <f t="shared" si="9"/>
         <v>71116.800000000003</v>
       </c>
-      <c r="R6" s="5">
-        <f t="shared" si="6"/>
+      <c r="S6" s="5">
+        <f t="shared" si="8"/>
         <v>51915264</v>
-      </c>
-      <c r="S6">
-        <v>20000</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -1542,50 +1556,52 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>46800</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>6240000</v>
+      </c>
+      <c r="J7" s="9">
         <v>2126.2249999999999</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" si="5"/>
+      <c r="K7" s="3">
+        <f t="shared" si="7"/>
         <v>663382.19999999995</v>
       </c>
-      <c r="J7" s="10">
+      <c r="L7" s="10">
         <f>'[1]CO2 calculations'!K8</f>
         <v>8164.7039999999997</v>
       </c>
-      <c r="K7" s="10">
-        <f t="shared" si="1"/>
+      <c r="M7" s="10">
+        <f t="shared" si="3"/>
         <v>2547387.648</v>
       </c>
-      <c r="L7" s="11">
-        <f t="shared" si="2"/>
+      <c r="N7" s="11">
+        <f t="shared" si="4"/>
         <v>2096287.7520000003</v>
       </c>
-      <c r="M7" s="11">
-        <f t="shared" si="3"/>
+      <c r="O7" s="11">
+        <f t="shared" si="5"/>
         <v>451099.89599999972</v>
       </c>
-      <c r="N7">
-        <v>150</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="P7" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C8</f>
         <v>56949.000000000007</v>
       </c>
-      <c r="P7" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q7" s="12">
+        <f t="shared" si="6"/>
         <v>17768088.000000004</v>
       </c>
-      <c r="Q7" s="14">
-        <f t="shared" si="7"/>
+      <c r="R7" s="14">
+        <f t="shared" si="9"/>
         <v>45559.200000000012</v>
       </c>
-      <c r="R7" s="12">
-        <f t="shared" si="6"/>
+      <c r="S7" s="12">
+        <f t="shared" si="8"/>
         <v>14214470.400000004</v>
-      </c>
-      <c r="S7">
-        <v>20000</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -1611,50 +1627,52 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>46800</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>6240000</v>
+      </c>
+      <c r="J8" s="3">
         <v>1486.35</v>
       </c>
-      <c r="I8" s="3">
-        <f t="shared" si="5"/>
+      <c r="K8" s="3">
+        <f t="shared" si="7"/>
         <v>463741.19999999995</v>
       </c>
-      <c r="J8" s="4">
+      <c r="L8" s="4">
         <f>'[1]CO2 calculations'!K9</f>
         <v>5707.5839999999998</v>
       </c>
-      <c r="K8" s="4">
-        <f t="shared" si="1"/>
-        <v>1780766.2079999999</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="2"/>
-        <v>1465422.192</v>
-      </c>
       <c r="M8" s="4">
         <f t="shared" si="3"/>
+        <v>1780766.2079999999</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="4"/>
+        <v>1465422.192</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="5"/>
         <v>315344.01599999983</v>
       </c>
-      <c r="N8">
-        <v>150</v>
-      </c>
-      <c r="O8" s="5">
+      <c r="P8" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C9</f>
         <v>34447.200000000004</v>
       </c>
-      <c r="P8" s="5">
-        <f t="shared" si="4"/>
+      <c r="Q8" s="5">
+        <f t="shared" si="6"/>
         <v>10747526.400000002</v>
       </c>
-      <c r="Q8" s="6">
-        <f t="shared" si="7"/>
+      <c r="R8" s="6">
+        <f t="shared" si="9"/>
         <v>27557.760000000006</v>
       </c>
-      <c r="R8" s="5">
-        <f t="shared" si="6"/>
+      <c r="S8" s="5">
+        <f t="shared" si="8"/>
         <v>8598021.1200000029</v>
-      </c>
-      <c r="S8">
-        <v>20000</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1680,50 +1698,52 @@
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>109500</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>14600000</v>
+      </c>
+      <c r="J9" s="9">
         <v>3010.7750000000001</v>
       </c>
-      <c r="I9" s="3">
-        <f t="shared" si="5"/>
+      <c r="K9" s="3">
+        <f t="shared" si="7"/>
         <v>2197865.75</v>
       </c>
-      <c r="J9" s="10">
+      <c r="L9" s="10">
         <f>'[1]CO2 calculations'!K10</f>
         <v>11561.376</v>
       </c>
-      <c r="K9" s="10">
-        <f t="shared" si="1"/>
+      <c r="M9" s="10">
+        <f t="shared" si="3"/>
         <v>8439804.4800000004</v>
       </c>
-      <c r="L9" s="11">
-        <f t="shared" si="2"/>
+      <c r="N9" s="11">
+        <f t="shared" si="4"/>
         <v>6945255.7700000014</v>
       </c>
-      <c r="M9" s="11">
-        <f t="shared" si="3"/>
+      <c r="O9" s="11">
+        <f t="shared" si="5"/>
         <v>1494548.709999999</v>
       </c>
-      <c r="N9">
-        <v>150</v>
-      </c>
-      <c r="O9" s="12">
+      <c r="P9" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C10</f>
         <v>99730.200000000012</v>
       </c>
-      <c r="P9" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q9" s="12">
+        <f t="shared" si="6"/>
         <v>72803046.000000015</v>
       </c>
-      <c r="Q9" s="14">
-        <f t="shared" si="7"/>
+      <c r="R9" s="14">
+        <f t="shared" si="9"/>
         <v>79784.160000000018</v>
       </c>
-      <c r="R9" s="12">
-        <f t="shared" si="6"/>
+      <c r="S9" s="12">
+        <f t="shared" si="8"/>
         <v>58242436.800000012</v>
-      </c>
-      <c r="S9">
-        <v>20000</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1749,50 +1769,52 @@
         <f t="shared" si="0"/>
         <v>1460</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>219000</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>29200000</v>
+      </c>
+      <c r="J10" s="3">
         <v>2274.7249999999999</v>
       </c>
-      <c r="I10" s="3">
-        <f t="shared" si="5"/>
+      <c r="K10" s="3">
+        <f t="shared" si="7"/>
         <v>3321098.5</v>
       </c>
-      <c r="J10" s="4">
+      <c r="L10" s="4">
         <f>'[1]CO2 calculations'!K11</f>
         <v>8734.9439999999995</v>
       </c>
-      <c r="K10" s="4">
-        <f t="shared" si="1"/>
-        <v>12753018.239999998</v>
-      </c>
-      <c r="L10" s="4">
-        <f t="shared" si="2"/>
-        <v>10494671.26</v>
-      </c>
       <c r="M10" s="4">
         <f t="shared" si="3"/>
+        <v>12753018.239999998</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="4"/>
+        <v>10494671.26</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="5"/>
         <v>2258346.9799999986</v>
       </c>
-      <c r="N10">
-        <v>150</v>
-      </c>
-      <c r="O10" s="5">
+      <c r="P10" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C11</f>
         <v>59727</v>
       </c>
-      <c r="P10" s="5">
-        <f t="shared" si="4"/>
+      <c r="Q10" s="5">
+        <f t="shared" si="6"/>
         <v>87201420</v>
       </c>
-      <c r="Q10" s="6">
-        <f t="shared" si="7"/>
+      <c r="R10" s="6">
+        <f t="shared" si="9"/>
         <v>47781.600000000006</v>
       </c>
-      <c r="R10" s="5">
-        <f t="shared" si="6"/>
+      <c r="S10" s="5">
+        <f t="shared" si="8"/>
         <v>69761136</v>
-      </c>
-      <c r="S10">
-        <v>20000</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1818,50 +1840,52 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>46800</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>6240000</v>
+      </c>
+      <c r="J11" s="9">
         <v>4227.6750000000002</v>
       </c>
-      <c r="I11" s="3">
-        <f t="shared" si="5"/>
+      <c r="K11" s="3">
+        <f t="shared" si="7"/>
         <v>1319034.6000000001</v>
       </c>
-      <c r="J11" s="10">
+      <c r="L11" s="10">
         <f>'[1]CO2 calculations'!K12</f>
         <v>16234.272000000001</v>
       </c>
-      <c r="K11" s="10">
-        <f t="shared" si="1"/>
+      <c r="M11" s="10">
+        <f t="shared" si="3"/>
         <v>5065092.8640000001</v>
       </c>
-      <c r="L11" s="11">
-        <f t="shared" si="2"/>
+      <c r="N11" s="11">
+        <f t="shared" si="4"/>
         <v>4168149.3360000006</v>
       </c>
-      <c r="M11" s="11">
-        <f t="shared" si="3"/>
+      <c r="O11" s="11">
+        <f t="shared" si="5"/>
         <v>896943.52799999947</v>
       </c>
-      <c r="N11">
-        <v>150</v>
-      </c>
-      <c r="O11" s="12">
+      <c r="P11" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C12</f>
         <v>148067.40000000002</v>
       </c>
-      <c r="P11" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q11" s="12">
+        <f t="shared" si="6"/>
         <v>46197028.800000004</v>
       </c>
-      <c r="Q11" s="14">
-        <f t="shared" si="7"/>
+      <c r="R11" s="14">
+        <f t="shared" si="9"/>
         <v>118453.92000000003</v>
       </c>
-      <c r="R11" s="12">
-        <f t="shared" si="6"/>
+      <c r="S11" s="12">
+        <f t="shared" si="8"/>
         <v>36957623.040000007</v>
-      </c>
-      <c r="S11">
-        <v>20000</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1887,50 +1911,52 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>46800</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>6240000</v>
+      </c>
+      <c r="J12" s="3">
         <v>3588.125</v>
       </c>
-      <c r="I12" s="3">
-        <f t="shared" si="5"/>
+      <c r="K12" s="3">
+        <f t="shared" si="7"/>
         <v>1119495</v>
       </c>
-      <c r="J12" s="4">
+      <c r="L12" s="4">
         <f>'[1]CO2 calculations'!K13</f>
         <v>13778.4</v>
       </c>
-      <c r="K12" s="4">
-        <f t="shared" si="1"/>
-        <v>4298860.8</v>
-      </c>
-      <c r="L12" s="4">
-        <f t="shared" si="2"/>
-        <v>3537604.2</v>
-      </c>
       <c r="M12" s="4">
         <f t="shared" si="3"/>
+        <v>4298860.8</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="4"/>
+        <v>3537604.2</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="5"/>
         <v>761256.59999999963</v>
       </c>
-      <c r="N12">
-        <v>150</v>
-      </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C13</f>
         <v>119454</v>
       </c>
-      <c r="P12" s="5">
-        <f t="shared" si="4"/>
+      <c r="Q12" s="5">
+        <f t="shared" si="6"/>
         <v>37269648</v>
       </c>
-      <c r="Q12" s="6">
-        <f t="shared" si="7"/>
+      <c r="R12" s="6">
+        <f t="shared" si="9"/>
         <v>95563.200000000012</v>
       </c>
-      <c r="R12" s="5">
-        <f t="shared" si="6"/>
+      <c r="S12" s="5">
+        <f t="shared" si="8"/>
         <v>29815718.400000002</v>
-      </c>
-      <c r="S12">
-        <v>20000</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1956,50 +1982,52 @@
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>109500</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>14600000</v>
+      </c>
+      <c r="J13" s="9">
         <v>5185.3999999999996</v>
       </c>
-      <c r="I13" s="3">
-        <f t="shared" si="5"/>
+      <c r="K13" s="3">
+        <f t="shared" si="7"/>
         <v>3785341.9999999995</v>
       </c>
-      <c r="J13" s="10">
+      <c r="L13" s="10">
         <f>'[1]CO2 calculations'!K14</f>
         <v>19911.935999999998</v>
       </c>
-      <c r="K13" s="10">
-        <f t="shared" si="1"/>
+      <c r="M13" s="10">
+        <f t="shared" si="3"/>
         <v>14535713.279999999</v>
       </c>
-      <c r="L13" s="11">
-        <f t="shared" si="2"/>
+      <c r="N13" s="11">
+        <f t="shared" si="4"/>
         <v>11961680.720000001</v>
       </c>
-      <c r="M13" s="11">
-        <f t="shared" si="3"/>
+      <c r="O13" s="11">
+        <f t="shared" si="5"/>
         <v>2574032.5599999987</v>
       </c>
-      <c r="N13">
-        <v>150</v>
-      </c>
-      <c r="O13" s="12">
+      <c r="P13" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C14</f>
         <v>194460</v>
       </c>
-      <c r="P13" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q13" s="12">
+        <f t="shared" si="6"/>
         <v>141955800</v>
       </c>
-      <c r="Q13" s="14">
-        <f t="shared" si="7"/>
+      <c r="R13" s="14">
+        <f t="shared" si="9"/>
         <v>155568</v>
       </c>
-      <c r="R13" s="12">
-        <f t="shared" si="6"/>
+      <c r="S13" s="12">
+        <f t="shared" si="8"/>
         <v>113564640</v>
-      </c>
-      <c r="S13">
-        <v>20000</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -2025,50 +2053,52 @@
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>109500</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>14600000</v>
+      </c>
+      <c r="J14" s="3">
         <v>6247.125</v>
       </c>
-      <c r="I14" s="3">
-        <f t="shared" si="5"/>
+      <c r="K14" s="3">
+        <f t="shared" si="7"/>
         <v>4560401.25</v>
       </c>
-      <c r="J14" s="4">
+      <c r="L14" s="4">
         <f>'[1]CO2 calculations'!K15</f>
         <v>23988.959999999999</v>
       </c>
-      <c r="K14" s="4">
-        <f t="shared" si="1"/>
-        <v>17511940.800000001</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="2"/>
-        <v>14410867.950000001</v>
-      </c>
       <c r="M14" s="4">
         <f t="shared" si="3"/>
+        <v>17511940.800000001</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="4"/>
+        <v>14410867.950000001</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="5"/>
         <v>3101072.8499999996</v>
       </c>
-      <c r="N14">
-        <v>150</v>
-      </c>
-      <c r="O14" s="5">
+      <c r="P14" s="5">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C15</f>
         <v>219184.2</v>
       </c>
-      <c r="P14" s="5">
-        <f t="shared" si="4"/>
+      <c r="Q14" s="5">
+        <f t="shared" si="6"/>
         <v>160004466</v>
       </c>
-      <c r="Q14" s="6">
-        <f t="shared" si="7"/>
+      <c r="R14" s="6">
+        <f t="shared" si="9"/>
         <v>175347.36000000002</v>
       </c>
-      <c r="R14" s="5">
-        <f t="shared" si="6"/>
+      <c r="S14" s="5">
+        <f t="shared" si="8"/>
         <v>128003572.80000001</v>
-      </c>
-      <c r="S14">
-        <v>20000</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -2094,50 +2124,52 @@
         <f t="shared" si="0"/>
         <v>730</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>109500</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>14600000</v>
+      </c>
+      <c r="J15" s="9">
         <v>5268.8</v>
       </c>
-      <c r="I15" s="3">
-        <f t="shared" si="5"/>
+      <c r="K15" s="3">
+        <f t="shared" si="7"/>
         <v>3846224</v>
       </c>
-      <c r="J15" s="10">
+      <c r="L15" s="10">
         <f>'[1]CO2 calculations'!K16</f>
         <v>20232.191999999999</v>
       </c>
-      <c r="K15" s="10">
-        <f t="shared" si="1"/>
+      <c r="M15" s="10">
+        <f t="shared" si="3"/>
         <v>14769500.16</v>
       </c>
-      <c r="L15" s="11">
-        <f t="shared" si="2"/>
+      <c r="N15" s="11">
+        <f t="shared" si="4"/>
         <v>12154067.840000002</v>
       </c>
-      <c r="M15" s="11">
-        <f t="shared" si="3"/>
+      <c r="O15" s="11">
+        <f t="shared" si="5"/>
         <v>2615432.3199999984</v>
       </c>
-      <c r="N15">
-        <v>150</v>
-      </c>
-      <c r="O15" s="12">
+      <c r="P15" s="12">
         <f>'[1]Aircraft Data'!$J$6*'[1]CO2 calculations'!C16</f>
         <v>186126.00000000003</v>
       </c>
-      <c r="P15" s="12">
-        <f t="shared" si="4"/>
+      <c r="Q15" s="12">
+        <f t="shared" si="6"/>
         <v>135871980.00000003</v>
       </c>
-      <c r="Q15" s="14">
-        <f t="shared" si="7"/>
+      <c r="R15" s="14">
+        <f t="shared" si="9"/>
         <v>148900.80000000002</v>
       </c>
-      <c r="R15" s="12">
-        <f t="shared" si="6"/>
+      <c r="S15" s="12">
+        <f t="shared" si="8"/>
         <v>108697584.00000003</v>
-      </c>
-      <c r="S15">
-        <v>20000</v>
       </c>
     </row>
   </sheetData>
@@ -2149,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F7E59F-12D8-455D-83B7-BC2E9A7794EF}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2161,16 +2193,16 @@
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -2193,41 +2225,41 @@
       <c r="G1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J1" s="17" t="s">
+      <c r="K1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="17" t="s">
+      <c r="N1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="O1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="S1" s="15" t="s">
         <v>12</v>
-      </c>
-      <c r="S1" s="15" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -2253,42 +2285,44 @@
         <f t="shared" ref="G2:G7" si="0">IF(F2="day",(E2*365*2),(E2*52*2))</f>
         <v>312</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="30">
+        <f t="shared" ref="H2:H7" si="1">301*G2</f>
+        <v>93912</v>
+      </c>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:I7" si="2">50000*G2</f>
+        <v>15600000</v>
+      </c>
+      <c r="J2" s="3">
         <v>103992.37</v>
       </c>
-      <c r="I2" s="3">
-        <f>G2*H2</f>
+      <c r="K2" s="3">
+        <f>G2*J2</f>
         <v>32445619.439999998</v>
       </c>
-      <c r="J2" s="4">
+      <c r="L2" s="4">
         <v>399330.70079999999</v>
       </c>
-      <c r="K2" s="4">
+      <c r="M2" s="4">
         <v>124591178.6496</v>
       </c>
-      <c r="L2" s="4">
+      <c r="N2" s="4">
         <v>102528157.43040001</v>
       </c>
-      <c r="M2" s="4">
+      <c r="O2" s="4">
         <v>22063021.219199985</v>
       </c>
-      <c r="N2" s="4">
-        <v>301</v>
-      </c>
-      <c r="O2" s="5">
+      <c r="P2" s="5">
         <v>1719304.2</v>
       </c>
-      <c r="P2" s="5">
+      <c r="Q2" s="5">
         <v>536422910.39999998</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="R2" s="6">
         <v>1375443</v>
       </c>
-      <c r="R2" s="5">
+      <c r="S2" s="5">
         <v>429138328</v>
-      </c>
-      <c r="S2" s="5">
-        <v>50000</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -2314,42 +2348,44 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="30">
+        <f t="shared" si="1"/>
+        <v>93912</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" si="2"/>
+        <v>15600000</v>
+      </c>
+      <c r="J3" s="9">
         <v>83634.09</v>
       </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I7" si="1">G3*H3</f>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K7" si="3">G3*J3</f>
         <v>26093836.079999998</v>
       </c>
-      <c r="J3" s="10">
+      <c r="L3" s="10">
         <v>321154.9056</v>
       </c>
-      <c r="K3" s="10">
+      <c r="M3" s="10">
         <v>100200330.54719999</v>
       </c>
-      <c r="L3" s="11">
+      <c r="N3" s="11">
         <v>82456522.012800008</v>
       </c>
-      <c r="M3" s="11">
+      <c r="O3" s="11">
         <v>17743808.534399986</v>
       </c>
-      <c r="N3" s="4">
-        <v>301</v>
-      </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>1326217.2</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>413779766.39999998</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="R3" s="13">
         <v>1060973</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>331023813</v>
-      </c>
-      <c r="S3" s="5">
-        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -2375,42 +2411,44 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="30">
+        <f t="shared" si="1"/>
+        <v>31304</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="2"/>
+        <v>5200000</v>
+      </c>
+      <c r="J4" s="3">
         <v>108618.22</v>
       </c>
-      <c r="I4" s="3">
-        <f t="shared" si="1"/>
+      <c r="K4" s="3">
+        <f t="shared" si="3"/>
         <v>11296294.880000001</v>
       </c>
-      <c r="J4" s="4">
+      <c r="L4" s="4">
         <v>417093.96480000002</v>
       </c>
-      <c r="K4" s="4">
+      <c r="M4" s="4">
         <v>43377772.339200005</v>
       </c>
-      <c r="L4" s="4">
+      <c r="N4" s="4">
         <v>35696291.820800006</v>
       </c>
-      <c r="M4" s="4">
+      <c r="O4" s="4">
         <v>7681480.5183999985</v>
       </c>
-      <c r="N4" s="4">
-        <v>301</v>
-      </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>1748751</v>
       </c>
-      <c r="P4" s="5">
+      <c r="Q4" s="5">
         <v>181870104</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="R4" s="6">
         <v>1399000</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <v>145496083</v>
-      </c>
-      <c r="S4" s="5">
-        <v>50000</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -2436,42 +2474,44 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="30">
+        <f t="shared" si="1"/>
+        <v>93912</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="2"/>
+        <v>15600000</v>
+      </c>
+      <c r="J5" s="9">
         <v>95974.47</v>
       </c>
-      <c r="I5" s="3">
-        <f t="shared" si="1"/>
+      <c r="K5" s="3">
+        <f t="shared" si="3"/>
         <v>29944034.640000001</v>
       </c>
-      <c r="J5" s="10">
+      <c r="L5" s="10">
         <v>368541.96480000002</v>
       </c>
-      <c r="K5" s="10">
+      <c r="M5" s="10">
         <v>114985093.0176</v>
       </c>
-      <c r="L5" s="11">
+      <c r="N5" s="11">
         <v>94623149.462400004</v>
       </c>
-      <c r="M5" s="11">
+      <c r="O5" s="11">
         <v>20361943.555199996</v>
       </c>
-      <c r="N5" s="4">
-        <v>301</v>
-      </c>
-      <c r="O5" s="12">
+      <c r="P5" s="12">
         <v>1703191.8</v>
       </c>
-      <c r="P5" s="12">
+      <c r="Q5" s="12">
         <v>531395841.60000002</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="R5" s="13">
         <v>1362553</v>
       </c>
-      <c r="R5" s="12">
+      <c r="S5" s="12">
         <v>425116673</v>
-      </c>
-      <c r="S5" s="5">
-        <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -2497,42 +2537,44 @@
         <f t="shared" si="0"/>
         <v>312</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="30">
+        <f t="shared" si="1"/>
+        <v>93912</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="2"/>
+        <v>15600000</v>
+      </c>
+      <c r="J6" s="3">
         <v>74692.789999999994</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" si="1"/>
+      <c r="K6" s="3">
+        <f t="shared" si="3"/>
         <v>23304150.479999997</v>
       </c>
-      <c r="J6" s="4">
+      <c r="L6" s="4">
         <v>286820.31359999994</v>
       </c>
-      <c r="K6" s="4">
+      <c r="M6" s="4">
         <v>89487937.843199983</v>
       </c>
-      <c r="L6" s="4">
+      <c r="N6" s="4">
         <v>73641115.516799986</v>
       </c>
-      <c r="M6" s="4">
+      <c r="O6" s="4">
         <v>15846822.326399997</v>
       </c>
-      <c r="N6" s="4">
-        <v>301</v>
-      </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <v>1382055</v>
       </c>
-      <c r="P6" s="5">
+      <c r="Q6" s="5">
         <v>431201160</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="R6" s="6">
         <v>1105644</v>
       </c>
-      <c r="R6" s="5">
+      <c r="S6" s="5">
         <v>344960928</v>
-      </c>
-      <c r="S6" s="5">
-        <v>50000</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -2558,67 +2600,69 @@
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="30">
+        <f t="shared" si="1"/>
+        <v>31304</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="2"/>
+        <v>5200000</v>
+      </c>
+      <c r="J7" s="9">
         <v>75655.91</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" si="1"/>
+      <c r="K7" s="3">
+        <f t="shared" si="3"/>
         <v>7868214.6400000006</v>
       </c>
-      <c r="J7" s="10">
+      <c r="L7" s="10">
         <v>290518.69439999998</v>
       </c>
-      <c r="K7" s="10">
+      <c r="M7" s="10">
         <v>30213944.217599999</v>
       </c>
-      <c r="L7" s="11">
+      <c r="N7" s="11">
         <v>24863558.262400001</v>
       </c>
-      <c r="M7" s="11">
+      <c r="O7" s="11">
         <v>5350385.9551999979</v>
       </c>
-      <c r="N7" s="4">
-        <v>301</v>
-      </c>
-      <c r="O7" s="12">
+      <c r="P7" s="12">
         <v>1185094.8</v>
       </c>
-      <c r="P7" s="12">
+      <c r="Q7" s="12">
         <v>123249859.2</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="R7" s="13">
         <v>948075</v>
       </c>
-      <c r="R7" s="12">
+      <c r="S7" s="12">
         <v>98599887</v>
       </c>
-      <c r="S7" s="5">
-        <v>50000</v>
-      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I10" s="3"/>
+      <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I13" s="3"/>
+      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I14" s="3"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2630,7 +2674,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2649,7 +2693,7 @@
         <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" t="s">
         <v>83</v>
@@ -2661,19 +2705,19 @@
         <v>85</v>
       </c>
       <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" t="s">
         <v>122</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>123</v>
-      </c>
-      <c r="J1" t="s">
-        <v>124</v>
       </c>
       <c r="K1" t="s">
         <v>88</v>
       </c>
       <c r="L1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -2687,7 +2731,7 @@
         <v>9172</v>
       </c>
       <c r="D2" s="20">
-        <f>SUM(Short_Haul!I:I)/1000</f>
+        <f>SUM(Short_Haul!K:K)/1000</f>
         <v>30966.037550000001</v>
       </c>
       <c r="E2">
@@ -2710,12 +2754,12 @@
         <v>129.24996384278259</v>
       </c>
       <c r="K2">
-        <f>SUM(Short_Haul!N2:N15)*2</f>
-        <v>4200</v>
+        <f>SUM(Short_Haul!H2:H15)</f>
+        <v>1375800</v>
       </c>
       <c r="L2">
-        <f>SUM(Short_Haul!S2:S15)/1000</f>
-        <v>280</v>
+        <f>SUM(Short_Haul!I2:I15)/1000</f>
+        <v>183440</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -2729,7 +2773,7 @@
         <v>1456</v>
       </c>
       <c r="D3" s="20">
-        <f>SUM(Long_Haul!I:I)/1000</f>
+        <f>SUM(Long_Haul!K:K)/1000</f>
         <v>130952.15015999998</v>
       </c>
       <c r="E3">
@@ -2752,12 +2796,12 @@
         <v>546.58663100994784</v>
       </c>
       <c r="K3">
-        <f>SUM(Long_Haul!N2:N7)*2</f>
-        <v>3612</v>
+        <f>SUM(Long_Haul!H2:H7)</f>
+        <v>438256</v>
       </c>
       <c r="L3">
-        <f>SUM(Long_Haul!S2:S7)/1000</f>
-        <v>300</v>
+        <f>SUM(Long_Haul!I2:I7)/1000</f>
+        <v>72800</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -2795,11 +2839,11 @@
       </c>
       <c r="K4">
         <f>SUM(K2:K3)</f>
-        <v>7812</v>
+        <v>1814056</v>
       </c>
       <c r="L4">
         <f>SUM(L2:L3)</f>
-        <v>580</v>
+        <v>256240</v>
       </c>
     </row>
   </sheetData>
@@ -2827,87 +2871,87 @@
   <sheetData>
     <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="22" t="s">
-        <v>102</v>
-      </c>
       <c r="D3" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="D4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>103</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>102</v>
-      </c>
       <c r="D5" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -2946,24 +2990,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>118</v>
       </c>
-      <c r="D1" t="s">
-        <v>119</v>
-      </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="26">
         <v>161918</v>
@@ -2983,7 +3027,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B3">
         <v>675.83</v>
@@ -3000,7 +3044,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4">
         <v>1814056</v>
@@ -3017,58 +3061,58 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="27">
         <f>299887.98*10268</f>
@@ -3089,7 +3133,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B9" s="27">
         <f>343760*10268</f>
@@ -3110,7 +3154,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B10" s="29">
         <f>(B9-B8)/B9</f>

</xml_diff>